<commit_message>
Published state of ETDataset for deploy November 2025
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/non_biogenic_waste.carrier.xlsx
+++ b/carriers_source_analyses/non_biogenic_waste.carrier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10905"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottevonm/Code/etdataset/carriers_source_analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyradehaan/github/etdataset/carriers_source_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1600E583-2A6C-D449-BDFE-9BF50B115914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CE335A-47B3-E94D-8043-225B1FC571F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26900" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10480" yWindow="28800" windowWidth="28800" windowHeight="18000" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>Source</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Date retrieved</t>
   </si>
   <si>
-    <t>Alexander Wirtz</t>
-  </si>
-  <si>
     <t>sustainable</t>
   </si>
   <si>
@@ -212,96 +209,115 @@
     <t>by definition</t>
   </si>
   <si>
-    <t>by assumption</t>
-  </si>
-  <si>
     <t>non_biogenic_waste</t>
   </si>
   <si>
-    <t>co2 per mj for waste (both biogenic and non-biogenic)</t>
-  </si>
-  <si>
-    <t>Share non-biogenic in total waste emission factor</t>
-  </si>
-  <si>
-    <t>Share non-biogenic in total waste energy content</t>
-  </si>
-  <si>
-    <t>co2 per mj non-biogenic waste (kg/GJ)</t>
-  </si>
-  <si>
-    <t>kg per mj</t>
-  </si>
-  <si>
-    <t>Agentschap NL (RVO)</t>
-  </si>
-  <si>
-    <t>p.10</t>
-  </si>
-  <si>
-    <r>
-      <t>Nederlandse lijst van energiedragers en standaard CO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- emissiefactoren </t>
-    </r>
-  </si>
-  <si>
-    <t>Agentschap NL/RVO</t>
-  </si>
-  <si>
     <t>NL</t>
   </si>
   <si>
-    <t>01-2012</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>05-01-2017</t>
-  </si>
-  <si>
-    <t>https://refman.energytransitionmodel.com/publications/2077</t>
-  </si>
-  <si>
-    <t>Note: The source does NOT assume that the co2 emission factor of biogenic waste is 0. Instead, they estimate the actual emissions from burning biogenic waste</t>
-  </si>
-  <si>
-    <t>RVO/Agentschap NL</t>
+    <t>TNO table:</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Assumptions:</t>
+  </si>
+  <si>
+    <t>Waste first value in D Other fuels is non-biogenic</t>
+  </si>
+  <si>
+    <t>Waste second value in D Other fuels is biogenic</t>
+  </si>
+  <si>
+    <t>non-biogenic waste</t>
+  </si>
+  <si>
+    <t>biogenic waste</t>
+  </si>
+  <si>
+    <t>CO2 (kg/MJ)</t>
+  </si>
+  <si>
+    <t>Density (MJ/kg)</t>
+  </si>
+  <si>
+    <t>Energy content and CO2 emission factor</t>
+  </si>
+  <si>
+    <t>TNO</t>
+  </si>
+  <si>
+    <t>Update of the Netherlands list of fuels in 2021</t>
+  </si>
+  <si>
+    <t>https://repository.tno.nl/SingleDoc?find=UID%202f9779a2-dd73-4f7f-9494-a44ddb7550d6</t>
+  </si>
+  <si>
+    <t>Claudia Valkenier</t>
+  </si>
+  <si>
+    <t>mj_per_kg</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>potential_co2_conversion_per_mj</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Costs per MJ</t>
+  </si>
+  <si>
+    <t>IEA</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>Advanced Biofuels – Potential for Cost Reduction</t>
+  </si>
+  <si>
+    <t>https://task39.ieabioenergy.com/wp-content/uploads/sites/37/2020/02/Advanced-Biofuels-Potential-for-Cost-Reduction-Final-Draft.pdf</t>
+  </si>
+  <si>
+    <t>IEA table pg  29</t>
+  </si>
+  <si>
+    <t>Waste costs as feedstock for methanol production are either zero or negative</t>
+  </si>
+  <si>
+    <t>therefore, costs for waste are assumed to be zero</t>
+  </si>
+  <si>
+    <t>costs per MJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="[$-413]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -473,16 +489,14 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <name val="Lettertype hoofdtekst"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="13">
@@ -559,7 +573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -839,556 +853,622 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="336">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="15" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="183" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="183" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="183" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="183" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="336">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1823,23 +1903,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>375478</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>220869</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>389314</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>77304</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>338436</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>144509</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F1139C7-2359-794A-8506-C1E5E33E078C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1855,8 +1935,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8525565" y="220869"/>
-          <a:ext cx="6374879" cy="10115826"/>
+          <a:off x="10634505" y="837363"/>
+          <a:ext cx="6702393" cy="7262091"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>156182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD63587-182D-D06F-A664-A474B694FB21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11252200" y="14376400"/>
+          <a:ext cx="7772400" cy="1857982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>355404</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>153168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3F6CA7B-2F86-AD48-A7D2-89811258BC83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11176000" y="8267700"/>
+          <a:ext cx="9105704" cy="6134868"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1869,7 +2037,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -1982,7 +2150,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover sheet"/>
@@ -2329,195 +2497,195 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="29" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" style="21" customWidth="1"/>
-    <col min="5" max="16384" width="10.85546875" style="21"/>
+    <col min="1" max="1" width="3.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="10.85546875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+    <row r="1" spans="1:4" s="22" customFormat="1">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="21">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>51</v>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>35</v>
+      <c r="C5" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="73" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="111"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="90"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="112"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="91"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="75" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="112"/>
+      <c r="D11" s="91"/>
     </row>
     <row r="12" spans="1:4" ht="17" thickBot="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="18" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="112"/>
+      <c r="D12" s="91"/>
     </row>
     <row r="13" spans="1:4" ht="17" thickBot="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="78" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="112"/>
+      <c r="D13" s="91"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="76" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="112"/>
+      <c r="D14" s="91"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="112"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="91"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="75" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="79" t="s">
+      <c r="C16" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="112"/>
+      <c r="D16" s="91"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="80" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="112"/>
+      <c r="D17" s="91"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="81" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="112"/>
+      <c r="D18" s="91"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="82" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="112"/>
+      <c r="D19" s="91"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="84" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="112"/>
+      <c r="D20" s="91"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="85" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="112"/>
+      <c r="D21" s="91"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="86" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="112"/>
+      <c r="D22" s="91"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="B23" s="83"/>
-      <c r="C23" s="87" t="s">
+      <c r="B23" s="70"/>
+      <c r="C23" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="112"/>
+      <c r="D23" s="91"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="113"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="115"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="94"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2530,150 +2698,156 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J11"/>
+  <dimension ref="B2:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="46" style="35" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="35" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" style="35" customWidth="1"/>
-    <col min="7" max="7" width="45" style="35" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="35" customWidth="1"/>
-    <col min="9" max="9" width="51.42578125" style="35" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" style="35" customWidth="1"/>
-    <col min="11" max="16384" width="10.85546875" style="35"/>
+    <col min="1" max="1" width="3.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="46" style="27" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" style="27" customWidth="1"/>
+    <col min="7" max="7" width="45" style="27" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="51.42578125" style="27" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" style="27" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-    </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="124" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="B2" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="140"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="127"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="143"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="130"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-    </row>
-    <row r="5" spans="2:10" ht="17" thickBot="1">
-      <c r="D5" s="33"/>
-    </row>
+      <c r="B4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="146"/>
+    </row>
+    <row r="5" spans="2:10" ht="17" thickBot="1"/>
     <row r="6" spans="2:10">
-      <c r="B6" s="36"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="37"/>
-    </row>
-    <row r="7" spans="2:10" s="41" customFormat="1" ht="19">
-      <c r="B7" s="88"/>
-      <c r="C7" s="19" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="2:10" s="34" customFormat="1" ht="19">
+      <c r="B7" s="75"/>
+      <c r="C7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="15"/>
+      <c r="I7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="90"/>
-    </row>
-    <row r="8" spans="2:10" s="41" customFormat="1" ht="19">
-      <c r="B8" s="23"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="42"/>
-    </row>
-    <row r="9" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
-      <c r="B9" s="23"/>
-      <c r="C9" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="42"/>
-    </row>
-    <row r="10" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
-      <c r="B10" s="23"/>
-      <c r="C10" s="94" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="J7" s="77"/>
+    </row>
+    <row r="8" spans="2:10" s="34" customFormat="1" ht="19">
+      <c r="B8" s="19"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="2:10" s="34" customFormat="1" ht="20" thickBot="1">
+      <c r="B9" s="19"/>
+      <c r="C9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="2:10" s="34" customFormat="1" ht="20" thickBot="1">
+      <c r="B10" s="19"/>
+      <c r="C10" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="101">
+      <c r="E10" s="127">
         <f>'Research data'!G6</f>
         <v>0</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="100" t="s">
+      <c r="F10" s="28"/>
+      <c r="G10" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="25"/>
+      <c r="I10" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="117" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="42"/>
-    </row>
-    <row r="11" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40"/>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="2:10" s="34" customFormat="1" ht="20" thickBot="1">
+      <c r="B11" s="19"/>
+      <c r="C11" s="125" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="102">
+        <f>'Research data'!G8</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="126" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="35"/>
+    </row>
+    <row r="12" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2719,179 +2893,237 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:L8"/>
+  <dimension ref="B1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="63" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="63" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="63" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="63" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="63" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="63" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="63" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="63" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="63" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="64" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="64" customWidth="1"/>
-    <col min="12" max="12" width="60" style="63" customWidth="1"/>
-    <col min="13" max="16384" width="10.85546875" style="63"/>
+    <col min="1" max="1" width="3.28515625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="53" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="53" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="53" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="53" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="53" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="53" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="53" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="54" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" style="54" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="54" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="54" customWidth="1"/>
+    <col min="14" max="14" width="60" style="53" customWidth="1"/>
+    <col min="15" max="16384" width="10.85546875" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17" thickBot="1"/>
-    <row r="2" spans="2:12">
-      <c r="B2" s="65"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-    </row>
-    <row r="3" spans="2:12" s="24" customFormat="1">
-      <c r="B3" s="23"/>
-      <c r="C3" s="93" t="s">
+    <row r="1" spans="2:14" ht="17" thickBot="1"/>
+    <row r="2" spans="2:14">
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="58"/>
+    </row>
+    <row r="3" spans="2:14" s="14" customFormat="1">
+      <c r="B3" s="19"/>
+      <c r="C3" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="93" t="s">
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93" t="s">
+      <c r="H3" s="78"/>
+      <c r="I3" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="51"/>
+      <c r="N3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="59"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="109"/>
+      <c r="M4" s="110"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="2:14" ht="17" thickBot="1">
+      <c r="B5" s="59"/>
+      <c r="C5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="2:14" ht="17" thickBot="1">
+      <c r="B6" s="59"/>
+      <c r="C6" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="102">
+        <v>0</v>
+      </c>
+      <c r="H6" s="114"/>
+      <c r="I6" s="115">
+        <v>1</v>
+      </c>
+      <c r="M6" s="112"/>
+      <c r="N6" s="95" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" s="5" customFormat="1" ht="17" thickBot="1">
+      <c r="B7" s="4"/>
+      <c r="C7" s="116" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="116" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="116" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="102">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="117"/>
+      <c r="L7" s="104">
+        <v>0</v>
+      </c>
+      <c r="M7" s="112"/>
+      <c r="N7" s="95"/>
+    </row>
+    <row r="8" spans="2:14" s="5" customFormat="1" ht="17" thickBot="1">
+      <c r="B8" s="4"/>
+      <c r="C8" s="118" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="102">
+        <f>ROUND(J8,3)</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="117"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="104">
+        <f>Notes!D11</f>
+        <v>10</v>
+      </c>
+      <c r="K8" s="150"/>
+      <c r="L8" s="150"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="95"/>
+    </row>
+    <row r="9" spans="2:14" s="5" customFormat="1" ht="17" thickBot="1">
+      <c r="B9" s="4"/>
+      <c r="C9" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="102">
+        <f>ROUND(J9,3)</f>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="H9" s="117"/>
+      <c r="J9" s="103">
+        <f>Notes!D10</f>
+        <v>9.1700000000000004E-2</v>
+      </c>
+      <c r="K9" s="151"/>
+      <c r="L9" s="151"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="95"/>
+    </row>
+    <row r="10" spans="2:14" ht="17" thickBot="1">
+      <c r="B10" s="59"/>
+      <c r="C10" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="2:12" ht="17" thickBot="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="2:12" ht="17" thickBot="1">
-      <c r="B6" s="69"/>
-      <c r="C6" s="102" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="102" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="102" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="43">
+      <c r="F10" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="105">
+        <f>I10</f>
         <v>0</v>
       </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="17">
-        <v>1</v>
-      </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="116" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" s="6" customFormat="1" ht="17" thickBot="1">
-      <c r="B7" s="5"/>
-      <c r="C7" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="109">
-        <f>J7</f>
+      <c r="I10" s="115">
         <v>0</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="17">
-        <v>0</v>
-      </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="116" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" s="6" customFormat="1" ht="17" thickBot="1">
-      <c r="B8" s="5"/>
-      <c r="C8" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="123">
-        <f>I8</f>
-        <v>8.3525531914893619E-2</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4">
-        <f>Notes!G10</f>
-        <v>8.3525531914893619E-2</v>
-      </c>
-      <c r="J8" s="17">
-        <v>0</v>
-      </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="116"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="2:14" ht="17" thickBot="1">
+      <c r="B11" s="120"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="123"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2906,175 +3138,174 @@
   </sheetPr>
   <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="44" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="44" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="44" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="44" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="5" style="44" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="44" customWidth="1"/>
-    <col min="8" max="10" width="12.140625" style="44" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="45" customWidth="1"/>
-    <col min="12" max="12" width="87.140625" style="44" customWidth="1"/>
-    <col min="13" max="16384" width="33.140625" style="44"/>
+    <col min="1" max="1" width="3.140625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="36" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="5" style="36" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="36" customWidth="1"/>
+    <col min="8" max="10" width="12.140625" style="36" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="37" customWidth="1"/>
+    <col min="12" max="12" width="87.140625" style="36" customWidth="1"/>
+    <col min="13" max="16384" width="33.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="17" thickBot="1"/>
     <row r="2" spans="2:12">
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="47"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="39"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="49"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="52"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="49"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="52"/>
+      <c r="B4" s="41"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55" t="s">
+      <c r="D5" s="45"/>
+      <c r="E5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55" t="s">
+      <c r="F5" s="45"/>
+      <c r="G5" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="K5" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="45" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="50"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="49"/>
-      <c r="C7" s="120" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="121" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="107"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="96"/>
+      <c r="E7" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="G7" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="96">
+        <v>2021</v>
+      </c>
+      <c r="I7" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="53" t="s">
+      <c r="J7" s="97">
+        <v>45898</v>
+      </c>
+      <c r="K7" s="98"/>
+      <c r="L7" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="62"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="49"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="105"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="62"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="85"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="49"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="62"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="147"/>
+      <c r="F9" s="147"/>
+      <c r="H9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="148">
+        <v>45901</v>
+      </c>
+      <c r="L9" s="149" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="49"/>
-      <c r="C10" s="110"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="108"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="L10" s="88"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1" xr:uid="{C1C92EB5-2EFF-CF45-B2E9-6EC95B594A1E}"/>
+    <hyperlink ref="L9" r:id="rId2" xr:uid="{DE993F1D-863A-5245-AF52-C443FF7E8360}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -3082,142 +3313,529 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:Q12"/>
+  <dimension ref="B1:AB41"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="D38" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="95" customWidth="1"/>
-    <col min="2" max="2" width="5" style="95" customWidth="1"/>
-    <col min="3" max="4" width="7" style="95"/>
-    <col min="5" max="5" width="10.28515625" style="95" customWidth="1"/>
-    <col min="6" max="6" width="49" style="95" customWidth="1"/>
-    <col min="7" max="16384" width="7" style="95"/>
+    <col min="1" max="1" width="5.7109375" style="80" customWidth="1"/>
+    <col min="2" max="2" width="5" style="80" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="80" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="80" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="80" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="80" customWidth="1"/>
+    <col min="7" max="16384" width="7" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="17" thickBot="1"/>
-    <row r="2" spans="2:17" s="24" customFormat="1">
-      <c r="B2" s="98"/>
-      <c r="C2" s="99" t="s">
+    <row r="1" spans="2:28" ht="17" thickBot="1"/>
+    <row r="2" spans="2:28" s="14" customFormat="1">
+      <c r="B2" s="82"/>
+      <c r="C2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="99" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99" t="s">
+      <c r="D2" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-    </row>
-    <row r="3" spans="2:17">
-      <c r="B3" s="96"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-    </row>
-    <row r="4" spans="2:17" customFormat="1">
-      <c r="B4" s="96"/>
-      <c r="C4" s="105" t="s">
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="137"/>
+    </row>
+    <row r="3" spans="2:28">
+      <c r="B3" s="81"/>
+      <c r="AB3" s="128"/>
+    </row>
+    <row r="4" spans="2:28" customFormat="1">
+      <c r="B4" s="81"/>
+      <c r="C4" s="129" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="131"/>
+      <c r="O4" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="130"/>
+      <c r="W4" s="130"/>
+      <c r="X4" s="130"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="132"/>
+    </row>
+    <row r="5" spans="2:28">
+      <c r="B5" s="81"/>
+      <c r="C5" s="130" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="130"/>
+      <c r="AB5" s="128"/>
+    </row>
+    <row r="6" spans="2:28">
+      <c r="B6" s="81"/>
+      <c r="C6" s="133" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="AB6" s="128"/>
+    </row>
+    <row r="7" spans="2:28">
+      <c r="B7" s="81"/>
+      <c r="C7" s="133" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="AB7" s="128"/>
+    </row>
+    <row r="8" spans="2:28">
+      <c r="B8" s="81"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="AB8" s="128"/>
+    </row>
+    <row r="9" spans="2:28">
+      <c r="B9" s="81"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="105"/>
-    </row>
-    <row r="5" spans="2:17" ht="17" thickBot="1">
-      <c r="D5" s="118" t="s">
+      <c r="F9" s="130"/>
+      <c r="G9" s="130"/>
+      <c r="H9" s="130"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
+      <c r="AB9" s="128"/>
+    </row>
+    <row r="10" spans="2:28">
+      <c r="B10" s="81"/>
+      <c r="C10" s="133" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="17" thickBot="1">
-      <c r="C6" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="118" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="119">
-        <v>106.1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="17" thickBot="1">
-      <c r="F7" s="118" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="119">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" ht="17" thickBot="1">
-      <c r="F8" s="118" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="119">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17">
-      <c r="F9" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="95">
-        <f>G6*G7/G8</f>
-        <v>83.52553191489362</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="F10" s="118" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="95">
-        <f>G9/1000</f>
-        <v>8.3525531914893619E-2</v>
-      </c>
-      <c r="H10" s="118" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" ht="51">
-      <c r="F12" s="122" t="s">
-        <v>66</v>
-      </c>
+      <c r="D10" s="96">
+        <f>91.7/1000</f>
+        <v>9.1700000000000004E-2</v>
+      </c>
+      <c r="E10" s="96">
+        <f>100/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="AB10" s="128"/>
+    </row>
+    <row r="11" spans="2:28">
+      <c r="B11" s="81"/>
+      <c r="C11" s="133" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="96">
+        <v>10</v>
+      </c>
+      <c r="E11" s="96">
+        <v>11.6</v>
+      </c>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="130"/>
+      <c r="AB11" s="128"/>
+    </row>
+    <row r="12" spans="2:28">
+      <c r="B12" s="81"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="AB12" s="128"/>
+    </row>
+    <row r="13" spans="2:28">
+      <c r="B13" s="81"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="AB13" s="128"/>
+    </row>
+    <row r="14" spans="2:28">
+      <c r="B14" s="81"/>
+      <c r="C14" s="129" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="AB14" s="128"/>
+    </row>
+    <row r="15" spans="2:28">
+      <c r="B15" s="81"/>
+      <c r="C15" s="130" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="AB15" s="128"/>
+    </row>
+    <row r="16" spans="2:28">
+      <c r="B16" s="81"/>
+      <c r="C16" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="130"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="130"/>
+      <c r="I16" s="130"/>
+      <c r="J16" s="130"/>
+      <c r="AB16" s="128"/>
+    </row>
+    <row r="17" spans="2:28">
+      <c r="B17" s="81"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="130"/>
+      <c r="AB17" s="128"/>
+    </row>
+    <row r="18" spans="2:28">
+      <c r="B18" s="81"/>
+      <c r="C18" s="130" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="130">
+        <v>0</v>
+      </c>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="130"/>
+      <c r="I18" s="130"/>
+      <c r="J18" s="130"/>
+      <c r="AB18" s="128"/>
+    </row>
+    <row r="19" spans="2:28">
+      <c r="B19" s="81"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="130"/>
+      <c r="I19" s="130"/>
+      <c r="J19" s="130"/>
+      <c r="AB19" s="128"/>
+    </row>
+    <row r="20" spans="2:28">
+      <c r="B20" s="81"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="130"/>
+      <c r="J20" s="130"/>
+      <c r="AB20" s="128"/>
+    </row>
+    <row r="21" spans="2:28">
+      <c r="B21" s="81"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="130"/>
+      <c r="H21" s="130"/>
+      <c r="I21" s="130"/>
+      <c r="J21" s="130"/>
+      <c r="AB21" s="128"/>
+    </row>
+    <row r="22" spans="2:28">
+      <c r="B22" s="81"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="130"/>
+      <c r="I22" s="130"/>
+      <c r="J22" s="130"/>
+      <c r="AB22" s="128"/>
+    </row>
+    <row r="23" spans="2:28">
+      <c r="B23" s="81"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
+      <c r="AB23" s="128"/>
+    </row>
+    <row r="24" spans="2:28">
+      <c r="B24" s="81"/>
+      <c r="C24" s="130"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="130"/>
+      <c r="I24" s="130"/>
+      <c r="J24" s="130"/>
+      <c r="AB24" s="128"/>
+    </row>
+    <row r="25" spans="2:28">
+      <c r="B25" s="81"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+      <c r="AB25" s="128"/>
+    </row>
+    <row r="26" spans="2:28">
+      <c r="B26" s="81"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="130"/>
+      <c r="J26" s="130"/>
+      <c r="AB26" s="128"/>
+    </row>
+    <row r="27" spans="2:28">
+      <c r="B27" s="81"/>
+      <c r="C27" s="130"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
+      <c r="G27" s="130"/>
+      <c r="H27" s="130"/>
+      <c r="I27" s="130"/>
+      <c r="J27" s="130"/>
+      <c r="AB27" s="128"/>
+    </row>
+    <row r="28" spans="2:28">
+      <c r="B28" s="81"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="130"/>
+      <c r="AB28" s="128"/>
+    </row>
+    <row r="29" spans="2:28">
+      <c r="B29" s="81"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="130"/>
+      <c r="J29" s="130"/>
+      <c r="AB29" s="128"/>
+    </row>
+    <row r="30" spans="2:28">
+      <c r="B30" s="81"/>
+      <c r="C30" s="130"/>
+      <c r="D30" s="130"/>
+      <c r="E30" s="130"/>
+      <c r="F30" s="130"/>
+      <c r="G30" s="130"/>
+      <c r="H30" s="130"/>
+      <c r="I30" s="130"/>
+      <c r="J30" s="130"/>
+      <c r="AB30" s="128"/>
+    </row>
+    <row r="31" spans="2:28">
+      <c r="B31" s="81"/>
+      <c r="C31" s="130"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="130"/>
+      <c r="F31" s="130"/>
+      <c r="G31" s="130"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="130"/>
+      <c r="J31" s="130"/>
+      <c r="AB31" s="128"/>
+    </row>
+    <row r="32" spans="2:28">
+      <c r="B32" s="81"/>
+      <c r="C32" s="130"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="130"/>
+      <c r="F32" s="130"/>
+      <c r="G32" s="130"/>
+      <c r="H32" s="130"/>
+      <c r="I32" s="130"/>
+      <c r="J32" s="130"/>
+      <c r="AB32" s="128"/>
+    </row>
+    <row r="33" spans="2:28">
+      <c r="B33" s="81"/>
+      <c r="AB33" s="128"/>
+    </row>
+    <row r="34" spans="2:28">
+      <c r="B34" s="81"/>
+      <c r="AB34" s="128"/>
+    </row>
+    <row r="35" spans="2:28">
+      <c r="B35" s="81"/>
+      <c r="AB35" s="128"/>
+    </row>
+    <row r="36" spans="2:28">
+      <c r="B36" s="81"/>
+      <c r="AB36" s="128"/>
+    </row>
+    <row r="37" spans="2:28">
+      <c r="B37" s="81"/>
+      <c r="AB37" s="128"/>
+    </row>
+    <row r="38" spans="2:28">
+      <c r="B38" s="81"/>
+      <c r="AB38" s="128"/>
+    </row>
+    <row r="39" spans="2:28">
+      <c r="B39" s="81"/>
+      <c r="AB39" s="128"/>
+    </row>
+    <row r="40" spans="2:28">
+      <c r="B40" s="81"/>
+      <c r="O40" s="147" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB40" s="128"/>
+    </row>
+    <row r="41" spans="2:28" ht="17" thickBot="1">
+      <c r="B41" s="134"/>
+      <c r="C41" s="135"/>
+      <c r="D41" s="135"/>
+      <c r="E41" s="135"/>
+      <c r="F41" s="135"/>
+      <c r="G41" s="135"/>
+      <c r="H41" s="135"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="135"/>
+      <c r="K41" s="135"/>
+      <c r="L41" s="135"/>
+      <c r="M41" s="135"/>
+      <c r="N41" s="135"/>
+      <c r="O41" s="135"/>
+      <c r="P41" s="135"/>
+      <c r="Q41" s="135"/>
+      <c r="R41" s="135"/>
+      <c r="S41" s="135"/>
+      <c r="T41" s="135"/>
+      <c r="U41" s="135"/>
+      <c r="V41" s="135"/>
+      <c r="W41" s="135"/>
+      <c r="X41" s="135"/>
+      <c r="Y41" s="135"/>
+      <c r="Z41" s="135"/>
+      <c r="AA41" s="135"/>
+      <c r="AB41" s="136"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>